<commit_message>
nhap mot chuoi, in ra chuoi dung mang
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v/code/ktlt/ktlt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDA0B7CD-0220-844D-97BE-C985F6746FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FFD870-A66C-8242-B409-61BA815561C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{026A610E-589E-2B40-9F9C-BA7647961D09}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">mov ah, 9 </t>
   </si>
@@ -245,6 +245,9 @@
       </rPr>
       <t>; đích&lt;-đích- nguồn</t>
     </r>
+  </si>
+  <si>
+    <t>kí tự nhập lưu trong al</t>
   </si>
 </sst>
 </file>
@@ -642,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF406800-DCF1-3547-9BE9-1BB46928305B}">
   <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="257" workbookViewId="0">
-      <selection activeCell="B24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="257" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -651,7 +654,7 @@
     <col min="1" max="1" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" style="4" customWidth="1"/>
@@ -681,6 +684,9 @@
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">

</xml_diff>